<commit_message>
archived old Excel files
</commit_message>
<xml_diff>
--- a/NMA- student counts by domain & intervention bundle.xlsx
+++ b/NMA- student counts by domain & intervention bundle.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sethb\Documents\Career\freelance\IRG\assignments\network meta-analysis\network-meta-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{385CE8D2-662D-4AAE-A995-2FC6FE96EC78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D46B51D7-41A6-4BF8-B842-DC857688D3B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{4269D852-3C15-4686-92AB-61DB45E99CAC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4269D852-3C15-4686-92AB-61DB45E99CAC}"/>
   </bookViews>
   <sheets>
-    <sheet name="WN" sheetId="7" r:id="rId1"/>
-    <sheet name="RN" sheetId="8" r:id="rId2"/>
+    <sheet name="Whole Numbers" sheetId="7" r:id="rId1"/>
+    <sheet name="Rational Numbers" sheetId="8" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">RN!$A$1:$G$49</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">WN!$A$1:$G$110</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Rational Numbers'!$A$1:$G$49</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Whole Numbers'!$A$1:$G$110</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -472,7 +472,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -495,7 +495,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -830,12 +829,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A4F7283-3DA4-4130-A163-925372471DBA}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:G109"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1" sqref="E1:E1048576"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -909,7 +907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" hidden="1">
+    <row r="4" spans="1:7">
       <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
@@ -932,7 +930,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:7" hidden="1">
+    <row r="5" spans="1:7">
       <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
@@ -952,7 +950,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" hidden="1">
+    <row r="6" spans="1:7">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
@@ -975,7 +973,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:7" hidden="1">
+    <row r="7" spans="1:7">
       <c r="A7" s="7" t="s">
         <v>4</v>
       </c>
@@ -1018,7 +1016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" hidden="1">
+    <row r="9" spans="1:7">
       <c r="A9" s="7" t="s">
         <v>8</v>
       </c>
@@ -1058,7 +1056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" hidden="1">
+    <row r="11" spans="1:7">
       <c r="A11" s="7" t="s">
         <v>9</v>
       </c>
@@ -1098,7 +1096,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" hidden="1">
+    <row r="13" spans="1:7">
       <c r="A13" s="7" t="s">
         <v>11</v>
       </c>
@@ -1138,7 +1136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" hidden="1">
+    <row r="15" spans="1:7">
       <c r="A15" s="5" t="s">
         <v>12</v>
       </c>
@@ -1181,7 +1179,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="17" spans="1:7" hidden="1">
+    <row r="17" spans="1:7">
       <c r="A17" s="7" t="s">
         <v>12</v>
       </c>
@@ -1224,7 +1222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" hidden="1">
+    <row r="19" spans="1:7">
       <c r="A19" s="7" t="s">
         <v>15</v>
       </c>
@@ -1264,7 +1262,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:7" hidden="1">
+    <row r="21" spans="1:7">
       <c r="A21" s="7" t="s">
         <v>16</v>
       </c>
@@ -1304,7 +1302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:7" hidden="1">
+    <row r="23" spans="1:7">
       <c r="A23" s="5" t="s">
         <v>17</v>
       </c>
@@ -1344,7 +1342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:7" hidden="1">
+    <row r="25" spans="1:7">
       <c r="A25" s="5" t="s">
         <v>17</v>
       </c>
@@ -1367,7 +1365,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="26" spans="1:7" hidden="1">
+    <row r="26" spans="1:7">
       <c r="A26" s="5" t="s">
         <v>17</v>
       </c>
@@ -1390,7 +1388,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="27" spans="1:7" hidden="1">
+    <row r="27" spans="1:7">
       <c r="A27" s="7" t="s">
         <v>17</v>
       </c>
@@ -1433,7 +1431,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:7" hidden="1">
+    <row r="29" spans="1:7">
       <c r="A29" s="7" t="s">
         <v>19</v>
       </c>
@@ -1493,7 +1491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:7" hidden="1">
+    <row r="32" spans="1:7">
       <c r="A32" s="5" t="s">
         <v>20</v>
       </c>
@@ -1516,7 +1514,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="33" spans="1:7" hidden="1">
+    <row r="33" spans="1:7">
       <c r="A33" s="5" t="s">
         <v>20</v>
       </c>
@@ -1536,7 +1534,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:7" hidden="1">
+    <row r="34" spans="1:7">
       <c r="A34" s="5" t="s">
         <v>20</v>
       </c>
@@ -1559,7 +1557,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="35" spans="1:7" hidden="1">
+    <row r="35" spans="1:7">
       <c r="A35" s="7" t="s">
         <v>20</v>
       </c>
@@ -1602,7 +1600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:7" hidden="1">
+    <row r="37" spans="1:7">
       <c r="A37" s="5" t="s">
         <v>22</v>
       </c>
@@ -1642,7 +1640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:7" hidden="1">
+    <row r="39" spans="1:7">
       <c r="A39" s="7" t="s">
         <v>22</v>
       </c>
@@ -1685,7 +1683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:7" hidden="1">
+    <row r="41" spans="1:7">
       <c r="A41" s="7" t="s">
         <v>23</v>
       </c>
@@ -1725,7 +1723,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:7" hidden="1">
+    <row r="43" spans="1:7">
       <c r="A43" s="7" t="s">
         <v>25</v>
       </c>
@@ -1765,7 +1763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:7" hidden="1">
+    <row r="45" spans="1:7">
       <c r="A45" s="7" t="s">
         <v>26</v>
       </c>
@@ -1805,7 +1803,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:7" hidden="1">
+    <row r="47" spans="1:7">
       <c r="A47" s="5" t="s">
         <v>27</v>
       </c>
@@ -1825,7 +1823,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:7" hidden="1">
+    <row r="48" spans="1:7">
       <c r="A48" s="5" t="s">
         <v>27</v>
       </c>
@@ -1908,7 +1906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:7" hidden="1">
+    <row r="52" spans="1:7">
       <c r="A52" s="5" t="s">
         <v>28</v>
       </c>
@@ -1931,7 +1929,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="53" spans="1:7" hidden="1">
+    <row r="53" spans="1:7">
       <c r="A53" s="5" t="s">
         <v>28</v>
       </c>
@@ -1951,7 +1949,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:7" hidden="1">
+    <row r="54" spans="1:7">
       <c r="A54" s="5" t="s">
         <v>28</v>
       </c>
@@ -1974,7 +1972,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="55" spans="1:7" hidden="1">
+    <row r="55" spans="1:7">
       <c r="A55" s="7" t="s">
         <v>28</v>
       </c>
@@ -2017,7 +2015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:7" hidden="1">
+    <row r="57" spans="1:7">
       <c r="A57" s="5" t="s">
         <v>31</v>
       </c>
@@ -2037,7 +2035,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:7" hidden="1">
+    <row r="58" spans="1:7">
       <c r="A58" s="5" t="s">
         <v>31</v>
       </c>
@@ -2060,7 +2058,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="59" spans="1:7" hidden="1">
+    <row r="59" spans="1:7">
       <c r="A59" s="7" t="s">
         <v>31</v>
       </c>
@@ -2103,7 +2101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:7" hidden="1">
+    <row r="61" spans="1:7">
       <c r="A61" s="5" t="s">
         <v>34</v>
       </c>
@@ -2143,7 +2141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:7" hidden="1">
+    <row r="63" spans="1:7">
       <c r="A63" s="7" t="s">
         <v>34</v>
       </c>
@@ -2186,7 +2184,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:7" hidden="1">
+    <row r="65" spans="1:7">
       <c r="A65" s="5" t="s">
         <v>35</v>
       </c>
@@ -2206,7 +2204,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:7" hidden="1">
+    <row r="66" spans="1:7">
       <c r="A66" s="5" t="s">
         <v>35</v>
       </c>
@@ -2229,7 +2227,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="67" spans="1:7" hidden="1">
+    <row r="67" spans="1:7">
       <c r="A67" s="7" t="s">
         <v>35</v>
       </c>
@@ -2272,7 +2270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:7" hidden="1">
+    <row r="69" spans="1:7">
       <c r="A69" s="7" t="s">
         <v>36</v>
       </c>
@@ -2312,7 +2310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:7" hidden="1">
+    <row r="71" spans="1:7">
       <c r="A71" s="7" t="s">
         <v>37</v>
       </c>
@@ -2352,7 +2350,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:7" hidden="1">
+    <row r="73" spans="1:7">
       <c r="A73" s="7" t="s">
         <v>38</v>
       </c>
@@ -2392,7 +2390,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:7" hidden="1">
+    <row r="75" spans="1:7">
       <c r="A75" s="7" t="s">
         <v>39</v>
       </c>
@@ -2452,7 +2450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:7" hidden="1">
+    <row r="78" spans="1:7">
       <c r="A78" s="5" t="s">
         <v>40</v>
       </c>
@@ -2475,7 +2473,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="79" spans="1:7" hidden="1">
+    <row r="79" spans="1:7">
       <c r="A79" s="5" t="s">
         <v>40</v>
       </c>
@@ -2495,7 +2493,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:7" hidden="1">
+    <row r="80" spans="1:7">
       <c r="A80" s="5" t="s">
         <v>40</v>
       </c>
@@ -2518,7 +2516,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="81" spans="1:7" hidden="1">
+    <row r="81" spans="1:7">
       <c r="A81" s="7" t="s">
         <v>40</v>
       </c>
@@ -2581,7 +2579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:7" hidden="1">
+    <row r="84" spans="1:7">
       <c r="A84" s="5" t="s">
         <v>42</v>
       </c>
@@ -2604,7 +2602,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="85" spans="1:7" hidden="1">
+    <row r="85" spans="1:7">
       <c r="A85" s="5" t="s">
         <v>42</v>
       </c>
@@ -2624,7 +2622,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="86" spans="1:7" hidden="1">
+    <row r="86" spans="1:7">
       <c r="A86" s="5" t="s">
         <v>42</v>
       </c>
@@ -2647,7 +2645,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="1:7" hidden="1">
+    <row r="87" spans="1:7">
       <c r="A87" s="5" t="s">
         <v>42</v>
       </c>
@@ -2690,7 +2688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:7" hidden="1">
+    <row r="89" spans="1:7">
       <c r="A89" s="7" t="s">
         <v>42</v>
       </c>
@@ -2733,7 +2731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:7" hidden="1">
+    <row r="91" spans="1:7">
       <c r="A91" s="5" t="s">
         <v>46</v>
       </c>
@@ -2776,7 +2774,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="93" spans="1:7" hidden="1">
+    <row r="93" spans="1:7">
       <c r="A93" s="7" t="s">
         <v>46</v>
       </c>
@@ -2819,7 +2817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:7" hidden="1">
+    <row r="95" spans="1:7">
       <c r="A95" s="7" t="s">
         <v>49</v>
       </c>
@@ -2859,7 +2857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:7" hidden="1">
+    <row r="97" spans="1:7">
       <c r="A97" s="5" t="s">
         <v>51</v>
       </c>
@@ -2902,7 +2900,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="99" spans="1:7" hidden="1">
+    <row r="99" spans="1:7">
       <c r="A99" s="7" t="s">
         <v>51</v>
       </c>
@@ -2942,7 +2940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:7" hidden="1">
+    <row r="101" spans="1:7">
       <c r="A101" s="7" t="s">
         <v>54</v>
       </c>
@@ -2982,7 +2980,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:7" hidden="1">
+    <row r="103" spans="1:7">
       <c r="A103" s="7" t="s">
         <v>55</v>
       </c>
@@ -3022,7 +3020,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:7" hidden="1">
+    <row r="105" spans="1:7">
       <c r="A105" s="5" t="s">
         <v>56</v>
       </c>
@@ -3065,7 +3063,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="107" spans="1:7" hidden="1">
+    <row r="107" spans="1:7">
       <c r="A107" s="7" t="s">
         <v>56</v>
       </c>
@@ -3105,7 +3103,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:7" hidden="1">
+    <row r="109" spans="1:7">
       <c r="A109" s="7" t="s">
         <v>59</v>
       </c>
@@ -3126,25 +3124,18 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G110" xr:uid="{0A4F7283-3DA4-4130-A163-925372471DBA}">
-    <filterColumn colId="5">
-      <filters blank="1">
-        <filter val="1"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:G110" xr:uid="{0A4F7283-3DA4-4130-A163-925372471DBA}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41275D72-607C-4EE2-98A3-187F1B0C7267}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E51" sqref="E51"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -3197,40 +3188,40 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" hidden="1">
+    <row r="3" spans="1:7">
       <c r="A3" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="18">
+      <c r="B3">
         <v>86186</v>
       </c>
-      <c r="C3" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="D3" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="18">
+      <c r="C3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3">
         <v>70</v>
       </c>
       <c r="F3" s="13">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" hidden="1">
+    <row r="4" spans="1:7">
       <c r="A4" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="18">
+      <c r="B4">
         <v>87223</v>
       </c>
-      <c r="C4" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="D4" s="18" t="s">
+      <c r="C4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" t="s">
         <v>64</v>
       </c>
-      <c r="E4" s="18">
+      <c r="E4">
         <v>69</v>
       </c>
       <c r="F4" s="13">
@@ -3244,36 +3235,36 @@
       <c r="A5" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B5" s="18">
+      <c r="B5">
         <v>87223</v>
       </c>
-      <c r="C5" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="D5" s="18" t="s">
+      <c r="C5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="18">
+      <c r="E5">
         <v>73</v>
       </c>
       <c r="F5" s="13">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" hidden="1">
+    <row r="6" spans="1:7">
       <c r="A6" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B6" s="18">
+      <c r="B6">
         <v>89765</v>
       </c>
-      <c r="C6" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="D6" s="18" t="s">
+      <c r="C6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" t="s">
         <v>43</v>
       </c>
-      <c r="E6" s="18">
+      <c r="E6">
         <v>69</v>
       </c>
       <c r="F6" s="13">
@@ -3283,7 +3274,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:7" hidden="1">
+    <row r="7" spans="1:7">
       <c r="A7" s="7" t="s">
         <v>63</v>
       </c>
@@ -3326,7 +3317,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" hidden="1">
+    <row r="9" spans="1:7">
       <c r="A9" s="7" t="s">
         <v>65</v>
       </c>
@@ -3366,40 +3357,40 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" hidden="1">
+    <row r="11" spans="1:7">
       <c r="A11" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" t="s">
         <v>67</v>
       </c>
-      <c r="C11" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="D11" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="18">
+      <c r="C11" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11">
         <v>70</v>
       </c>
       <c r="F11" s="13">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" hidden="1">
+    <row r="12" spans="1:7">
       <c r="A12" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B12" s="18">
+      <c r="B12">
         <v>89813</v>
       </c>
-      <c r="C12" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="D12" s="18" t="s">
+      <c r="C12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" t="s">
         <v>24</v>
       </c>
-      <c r="E12" s="18">
+      <c r="E12">
         <v>72</v>
       </c>
       <c r="F12" s="13">
@@ -3409,7 +3400,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="13" spans="1:7" hidden="1">
+    <row r="13" spans="1:7">
       <c r="A13" s="7" t="s">
         <v>66</v>
       </c>
@@ -3452,7 +3443,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" hidden="1">
+    <row r="15" spans="1:7">
       <c r="A15" s="7" t="s">
         <v>39</v>
       </c>
@@ -3492,7 +3483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" hidden="1">
+    <row r="17" spans="1:7">
       <c r="A17" s="7" t="s">
         <v>68</v>
       </c>
@@ -3532,7 +3523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" hidden="1">
+    <row r="19" spans="1:7">
       <c r="A19" s="7" t="s">
         <v>69</v>
       </c>
@@ -3572,7 +3563,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:7" hidden="1">
+    <row r="21" spans="1:7">
       <c r="A21" s="7" t="s">
         <v>70</v>
       </c>
@@ -3612,40 +3603,40 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:7" hidden="1">
+    <row r="23" spans="1:7">
       <c r="A23" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B23" s="18">
+      <c r="B23">
         <v>88710</v>
       </c>
-      <c r="C23" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="D23" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="E23" s="18">
+      <c r="C23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23">
         <v>29</v>
       </c>
       <c r="F23" s="13">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:7" hidden="1">
+    <row r="24" spans="1:7">
       <c r="A24" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B24" s="18" t="s">
+      <c r="B24" t="s">
         <v>73</v>
       </c>
-      <c r="C24" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="D24" s="18" t="s">
+      <c r="C24" t="s">
+        <v>61</v>
+      </c>
+      <c r="D24" t="s">
         <v>43</v>
       </c>
-      <c r="E24" s="18">
+      <c r="E24">
         <v>26</v>
       </c>
       <c r="F24" s="13">
@@ -3655,7 +3646,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:7" hidden="1">
+    <row r="25" spans="1:7">
       <c r="A25" s="7" t="s">
         <v>72</v>
       </c>
@@ -3702,36 +3693,36 @@
       <c r="A27" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B27" s="18">
+      <c r="B27">
         <v>88692</v>
       </c>
-      <c r="C27" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="D27" s="18" t="s">
+      <c r="C27" t="s">
+        <v>62</v>
+      </c>
+      <c r="D27" t="s">
         <v>43</v>
       </c>
-      <c r="E27" s="18">
+      <c r="E27">
         <v>45</v>
       </c>
       <c r="F27" s="13">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:7" hidden="1">
+    <row r="28" spans="1:7">
       <c r="A28" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B28" s="18">
+      <c r="B28">
         <v>88693</v>
       </c>
-      <c r="C28" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="D28" s="18" t="s">
+      <c r="C28" t="s">
+        <v>61</v>
+      </c>
+      <c r="D28" t="s">
         <v>64</v>
       </c>
-      <c r="E28" s="18">
+      <c r="E28">
         <v>45</v>
       </c>
       <c r="F28" s="13">
@@ -3741,40 +3732,40 @@
         <v>85</v>
       </c>
     </row>
-    <row r="29" spans="1:7" hidden="1">
+    <row r="29" spans="1:7">
       <c r="A29" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B29" s="18">
+      <c r="B29">
         <v>88693</v>
       </c>
-      <c r="C29" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="D29" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="E29" s="18">
+      <c r="C29" t="s">
+        <v>62</v>
+      </c>
+      <c r="D29" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29">
         <v>52</v>
       </c>
       <c r="F29" s="13">
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:7" hidden="1">
+    <row r="30" spans="1:7">
       <c r="A30" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B30" s="18" t="s">
+      <c r="B30" t="s">
         <v>75</v>
       </c>
-      <c r="C30" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="D30" s="18" t="s">
+      <c r="C30" t="s">
+        <v>61</v>
+      </c>
+      <c r="D30" t="s">
         <v>43</v>
       </c>
-      <c r="E30" s="18">
+      <c r="E30">
         <v>46</v>
       </c>
       <c r="F30" s="13">
@@ -3784,7 +3775,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="31" spans="1:7" hidden="1">
+    <row r="31" spans="1:7">
       <c r="A31" s="7" t="s">
         <v>74</v>
       </c>
@@ -3827,40 +3818,40 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:7" hidden="1">
+    <row r="33" spans="1:7">
       <c r="A33" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B33" s="18">
+      <c r="B33">
         <v>88775</v>
       </c>
-      <c r="C33" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="D33" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="E33" s="18">
+      <c r="C33" t="s">
+        <v>62</v>
+      </c>
+      <c r="D33" t="s">
+        <v>7</v>
+      </c>
+      <c r="E33">
         <v>76</v>
       </c>
       <c r="F33" s="13">
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:7" hidden="1">
+    <row r="34" spans="1:7">
       <c r="A34" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B34" s="18">
+      <c r="B34">
         <v>89179</v>
       </c>
-      <c r="C34" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="D34" s="18" t="s">
+      <c r="C34" t="s">
+        <v>61</v>
+      </c>
+      <c r="D34" t="s">
         <v>64</v>
       </c>
-      <c r="E34" s="18">
+      <c r="E34">
         <v>73</v>
       </c>
       <c r="F34" s="13">
@@ -3870,7 +3861,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="35" spans="1:7" hidden="1">
+    <row r="35" spans="1:7">
       <c r="A35" s="7" t="s">
         <v>76</v>
       </c>
@@ -3913,20 +3904,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:7" hidden="1">
+    <row r="37" spans="1:7">
       <c r="A37" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B37" s="18">
+      <c r="B37">
         <v>82135</v>
       </c>
-      <c r="C37" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="D37" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="E37" s="18">
+      <c r="C37" t="s">
+        <v>62</v>
+      </c>
+      <c r="D37" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37">
         <v>80</v>
       </c>
       <c r="F37" s="13">
@@ -3937,36 +3928,36 @@
       <c r="A38" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B38" s="18">
+      <c r="B38">
         <v>86189</v>
       </c>
-      <c r="C38" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="D38" s="18" t="s">
+      <c r="C38" t="s">
+        <v>61</v>
+      </c>
+      <c r="D38" t="s">
         <v>64</v>
       </c>
-      <c r="E38" s="18">
+      <c r="E38">
         <v>84</v>
       </c>
       <c r="F38" s="13">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:7" hidden="1">
+    <row r="39" spans="1:7">
       <c r="A39" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B39" s="18">
+      <c r="B39">
         <v>86189</v>
       </c>
-      <c r="C39" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="D39" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="E39" s="18">
+      <c r="C39" t="s">
+        <v>62</v>
+      </c>
+      <c r="D39" t="s">
+        <v>7</v>
+      </c>
+      <c r="E39">
         <v>80</v>
       </c>
       <c r="F39" s="13">
@@ -3976,20 +3967,20 @@
         <v>85</v>
       </c>
     </row>
-    <row r="40" spans="1:7" hidden="1">
+    <row r="40" spans="1:7">
       <c r="A40" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B40" s="18">
+      <c r="B40">
         <v>87221</v>
       </c>
-      <c r="C40" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="D40" s="18" t="s">
+      <c r="C40" t="s">
+        <v>61</v>
+      </c>
+      <c r="D40" t="s">
         <v>64</v>
       </c>
-      <c r="E40" s="18">
+      <c r="E40">
         <v>84</v>
       </c>
       <c r="F40" s="13">
@@ -3999,7 +3990,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="41" spans="1:7" hidden="1">
+    <row r="41" spans="1:7">
       <c r="A41" s="7" t="s">
         <v>77</v>
       </c>
@@ -4042,7 +4033,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:7" hidden="1">
+    <row r="43" spans="1:7">
       <c r="A43" s="7" t="s">
         <v>79</v>
       </c>
@@ -4082,7 +4073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:7" hidden="1">
+    <row r="45" spans="1:7">
       <c r="A45" s="7" t="s">
         <v>80</v>
       </c>
@@ -4106,56 +4097,56 @@
       <c r="A46" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B46" s="18" t="s">
+      <c r="B46" t="s">
         <v>83</v>
       </c>
-      <c r="C46" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="D46" s="18" t="s">
+      <c r="C46" t="s">
+        <v>61</v>
+      </c>
+      <c r="D46" t="s">
         <v>43</v>
       </c>
-      <c r="E46" s="18">
+      <c r="E46">
         <v>44</v>
       </c>
       <c r="F46" s="13">
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:7" hidden="1">
+    <row r="47" spans="1:7">
       <c r="A47" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B47" s="18" t="s">
+      <c r="B47" t="s">
         <v>83</v>
       </c>
-      <c r="C47" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="D47" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="E47" s="18">
+      <c r="C47" t="s">
+        <v>62</v>
+      </c>
+      <c r="D47" t="s">
+        <v>7</v>
+      </c>
+      <c r="E47">
         <v>50</v>
       </c>
       <c r="F47" s="13">
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:7" hidden="1">
+    <row r="48" spans="1:7">
       <c r="A48" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B48" s="18" t="s">
+      <c r="B48" t="s">
         <v>84</v>
       </c>
-      <c r="C48" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="D48" s="18" t="s">
+      <c r="C48" t="s">
+        <v>61</v>
+      </c>
+      <c r="D48" t="s">
         <v>43</v>
       </c>
-      <c r="E48" s="18">
+      <c r="E48">
         <v>48</v>
       </c>
       <c r="F48" s="13">
@@ -4165,7 +4156,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="49" spans="1:7" hidden="1">
+    <row r="49" spans="1:7">
       <c r="A49" s="7" t="s">
         <v>82</v>
       </c>
@@ -4189,13 +4180,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G49" xr:uid="{41275D72-607C-4EE2-98A3-187F1B0C7267}">
-    <filterColumn colId="5">
-      <filters>
-        <filter val="1"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:G49" xr:uid="{41275D72-607C-4EE2-98A3-187F1B0C7267}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>